<commit_message>
SAL jurnal rsa + spm , tabel akun2 + pejabat
</commit_message>
<xml_diff>
--- a/data_pendukung/Nama Pejabat (1).xlsx
+++ b/data_pendukung/Nama Pejabat (1).xlsx
@@ -9,22 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 5" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="GABUNG" sheetId="3" r:id="rId1"/>
+    <sheet name="Table 5" sheetId="1" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Table 2'!$A$3:$D$19</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Table 5'!$A$3:$C$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GABUNG!$A$3:$C$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Table 2'!$A$3:$D$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Table 5'!$A$3:$C$21</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="156">
   <si>
     <t xml:space="preserve">No.
 </t>
@@ -219,6 +221,9 @@
 </t>
   </si>
   <si>
+    <t>Penyusun Laporan</t>
+  </si>
+  <si>
     <t>NIP</t>
   </si>
   <si>
@@ -516,10 +521,109 @@
     <t>197811162001121001</t>
   </si>
   <si>
-    <t>jabatan</t>
+    <t>'H.7.1976050609082001</t>
+  </si>
+  <si>
+    <t>Inda Hayuningtyas</t>
+  </si>
+  <si>
+    <t>'H.7.1986012409082011</t>
+  </si>
+  <si>
+    <t>Suryani</t>
+  </si>
+  <si>
+    <t>'H.7.1988111009082025</t>
+  </si>
+  <si>
+    <t>Nova Rosyada</t>
+  </si>
+  <si>
+    <t>'H.7.1981121709082005</t>
+  </si>
+  <si>
+    <t>Yusmida</t>
+  </si>
+  <si>
+    <t>'H.7.1987112609082017</t>
+  </si>
+  <si>
+    <t>Novita Anugrah Listiyana</t>
+  </si>
+  <si>
+    <t>'H.7.1988060609082021</t>
+  </si>
+  <si>
+    <t>Domas Titis Anggit</t>
+  </si>
+  <si>
+    <t>'H.7.1988052309082020</t>
+  </si>
+  <si>
+    <t>Resti Fitria Dewi</t>
+  </si>
+  <si>
+    <t>'H.7.1978021709082002</t>
+  </si>
+  <si>
+    <t>Feb Arylla Endra Devi</t>
+  </si>
+  <si>
+    <t>Sari Widyastuti, S.T.</t>
+  </si>
+  <si>
+    <t>198401110214012081</t>
+  </si>
+  <si>
+    <t>Maharani Wulan Sari, S.E.</t>
+  </si>
+  <si>
+    <t>Murni Julianti, S.E.</t>
+  </si>
+  <si>
+    <t>199207180214062528</t>
+  </si>
+  <si>
+    <t>198607150214062527</t>
+  </si>
+  <si>
+    <t>Choiriyah, SE</t>
+  </si>
+  <si>
+    <t>198508112010122002</t>
+  </si>
+  <si>
+    <t>Syaidatina Zahroh, S.E.</t>
+  </si>
+  <si>
+    <t>199209140216012025</t>
+  </si>
+  <si>
+    <t>'H.7.1984050410061031</t>
+  </si>
+  <si>
+    <t>Sri Agung Wibowo</t>
+  </si>
+  <si>
+    <t>'H.7.1985082610062038</t>
+  </si>
+  <si>
+    <t>Idha Rosalina</t>
+  </si>
+  <si>
+    <t>Jabatan</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>ppk</t>
+  </si>
+  <si>
+    <t>operator</t>
   </si>
   <si>
     <t>kpa</t>
@@ -533,7 +637,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_);\-#,##0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
@@ -577,6 +681,35 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -592,7 +725,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -639,15 +772,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -655,7 +779,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -672,12 +796,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -716,7 +834,31 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1024,10 +1166,1259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="52.83203125" customWidth="1"/>
+    <col min="4" max="4" width="36.5" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3">
+        <v>41</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3">
+        <v>51</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="4">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4">
+        <v>44</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4">
+        <v>82</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4">
+        <v>62</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4">
+        <v>41</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>18</v>
+      </c>
+      <c r="B25" s="4">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4">
+        <v>61</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>18</v>
+      </c>
+      <c r="B27" s="4">
+        <v>91</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4">
+        <v>81</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>19</v>
+      </c>
+      <c r="B29" s="3">
+        <v>11</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>20</v>
+      </c>
+      <c r="B30" s="3">
+        <v>12</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3">
+        <v>13</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3">
+        <v>14</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3">
+        <v>15</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3">
+        <v>16</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3">
+        <v>17</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3">
+        <v>18</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>27</v>
+      </c>
+      <c r="B37" s="3">
+        <v>19</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>28</v>
+      </c>
+      <c r="B38" s="3">
+        <v>20</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>29</v>
+      </c>
+      <c r="B39" s="3">
+        <v>21</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>30</v>
+      </c>
+      <c r="B40" s="3">
+        <v>31</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>31</v>
+      </c>
+      <c r="B41" s="3">
+        <v>32</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3">
+        <v>71</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3">
+        <v>72</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>34</v>
+      </c>
+      <c r="B44" s="3">
+        <v>51</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="21"/>
+      <c r="E44" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>35</v>
+      </c>
+      <c r="B45" s="4">
+        <v>42</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" s="21"/>
+      <c r="E45" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>35</v>
+      </c>
+      <c r="B46" s="4">
+        <v>44</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="21"/>
+      <c r="E46" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>35</v>
+      </c>
+      <c r="B47" s="4">
+        <v>82</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>35</v>
+      </c>
+      <c r="B48" s="4">
+        <v>62</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>36</v>
+      </c>
+      <c r="B49" s="4">
+        <v>41</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>36</v>
+      </c>
+      <c r="B50" s="4">
+        <v>43</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>36</v>
+      </c>
+      <c r="B51" s="4">
+        <v>61</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>36</v>
+      </c>
+      <c r="B52" s="4">
+        <v>91</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>36</v>
+      </c>
+      <c r="B53" s="4">
+        <v>81</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="21"/>
+      <c r="E53" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>37</v>
+      </c>
+      <c r="B54" s="3">
+        <v>11</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>38</v>
+      </c>
+      <c r="B55" s="3">
+        <v>12</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>39</v>
+      </c>
+      <c r="B56" s="3">
+        <v>13</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>40</v>
+      </c>
+      <c r="B57" s="3">
+        <v>14</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>41</v>
+      </c>
+      <c r="B58" s="3">
+        <v>15</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>42</v>
+      </c>
+      <c r="B59" s="3">
+        <v>16</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>43</v>
+      </c>
+      <c r="B60" s="3">
+        <v>17</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>44</v>
+      </c>
+      <c r="B61" s="3">
+        <v>18</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>45</v>
+      </c>
+      <c r="B62" s="3">
+        <v>19</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>46</v>
+      </c>
+      <c r="B63" s="3">
+        <v>20</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>47</v>
+      </c>
+      <c r="B64" s="3">
+        <v>21</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>48</v>
+      </c>
+      <c r="B65" s="3">
+        <v>31</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>49</v>
+      </c>
+      <c r="B66" s="3">
+        <v>32</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>50</v>
+      </c>
+      <c r="B67" s="3">
+        <v>71</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>51</v>
+      </c>
+      <c r="B68" s="3">
+        <v>72</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>52</v>
+      </c>
+      <c r="B69" s="3">
+        <v>51</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>53</v>
+      </c>
+      <c r="B70" s="3">
+        <v>41</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>54</v>
+      </c>
+      <c r="B71" s="3">
+        <v>42</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>55</v>
+      </c>
+      <c r="B72" s="3">
+        <v>43</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>56</v>
+      </c>
+      <c r="B73" s="3">
+        <v>44</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>57</v>
+      </c>
+      <c r="B74" s="3">
+        <v>62</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>58</v>
+      </c>
+      <c r="B75" s="3">
+        <v>61</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74803149606299213" right="0.28000000000000003" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1039,33 +2430,33 @@
     <col min="5" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:7" s="9" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1075,15 +2466,17 @@
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1093,15 +2486,17 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D5" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1111,15 +2506,17 @@
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D6" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1129,15 +2526,17 @@
       <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1147,15 +2546,17 @@
       <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D8" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1165,15 +2566,17 @@
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1183,15 +2586,17 @@
       <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1201,15 +2606,17 @@
       <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D11" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1219,15 +2626,17 @@
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D12" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1237,15 +2646,17 @@
       <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D13" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1255,15 +2666,18 @@
       <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D14" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1273,15 +2687,17 @@
       <c r="C15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="D15" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1291,15 +2707,17 @@
       <c r="C16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="D16" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1309,15 +2727,17 @@
       <c r="C17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="D17" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1327,13 +2747,15 @@
       <c r="C18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="7"/>
+      <c r="D18" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -1345,13 +2767,11 @@
       <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="7"/>
+      <c r="D19" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1363,13 +2783,11 @@
       <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="7"/>
+      <c r="D20" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1381,45 +2799,42 @@
       <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="7"/>
+      <c r="D21" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.74803149606299213" right="0.28000000000000003" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="90" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="49.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="33.5" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1427,387 +2842,318 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+        <v>43</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+        <v>45</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+        <v>46</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+        <v>47</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+        <v>48</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
+        <v>50</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+        <v>52</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+        <v>54</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+        <v>56</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
+        <v>58</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="12">
+        <v>59</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="12">
+        <v>61</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A17" s="12">
+        <v>62</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.2">
-      <c r="A18" s="12">
+        <v>64</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="17" t="s">
+      <c r="D25" s="16" t="s">
         <v>83</v>
-      </c>
-      <c r="E18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="12">
-        <v>16</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A20" s="12">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="12">
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
-        <v>20</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
-        <v>21</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" s="12">
-        <v>22</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>